<commit_message>
updated to recommended caps
</commit_message>
<xml_diff>
--- a/sulu-reg/sulu_reg_bom.xlsx
+++ b/sulu-reg/sulu_reg_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\source\repos\scum-dev-board\sulu-reg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D3743-0E3B-4557-A7F0-AEFF68A38A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2634F6A1-007B-4B80-B115-479EEFF4C22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="5460" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -96,33 +96,18 @@
     <t>https://www.digikey.com/en/products/detail/tdk-invensense/ICM-20948/6623535</t>
   </si>
   <si>
-    <t>C_1.1_OUT1, C_1.8_OUT2</t>
-  </si>
-  <si>
     <t>BT1</t>
   </si>
   <si>
-    <t>C_1.1_IN1, C_1.8_IN2</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05B104KQ5NNNC/3887169</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05A106MP8NUB8/5961314</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 10V X5R 0402</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BH1000G/140383</t>
   </si>
   <si>
     <t>Battery Holder (Open) Coin, 24.5mm 1 Cell PC Pin</t>
   </si>
   <si>
-    <t>Coin, 24.5mm Lithium Manganese Dioxide Battery Non-Rechargeable (Primary)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/ablic-u-s-a-inc/S-85S1AB18-I6T1U/9489538</t>
   </si>
   <si>
@@ -156,30 +141,9 @@
     <t>Accelerometer, Gyroscope, Magnetometer, 9 Axis Sensor I²C, SPI Output</t>
   </si>
   <si>
-    <t>CAP CER 100UF 2.5V X5R 0805</t>
-  </si>
-  <si>
-    <t>100 µF ±20% 2.5V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>GRM21BR60E107ME15L</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR60E107ME15L/6155809</t>
-  </si>
-  <si>
     <t>BH1000G</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR-2477-JAUCH-(IB)/9561010</t>
-  </si>
-  <si>
-    <t>BATT LITHIUM COIN 3.0V</t>
-  </si>
-  <si>
-    <t>CR 2477 JAUCH (IB)</t>
-  </si>
-  <si>
     <t>S-85S1AB18-I6T1U</t>
   </si>
   <si>
@@ -225,9 +189,6 @@
     <t>RMCF0402FT66K5</t>
   </si>
   <si>
-    <t>10 µF ±20% 10V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
@@ -238,6 +199,33 @@
   </si>
   <si>
     <t>FIXED IND 2.2UH 1.1A 270MOHM SMD</t>
+  </si>
+  <si>
+    <t>C_1.1_OUT1, C_1.8_OUT2, C_1.1_IN1, C_1.8_IN2</t>
+  </si>
+  <si>
+    <t>GRM155R60J106ME15D</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t>10 µF ±20% 6.3V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>SCuM QFN</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -735,11 +723,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1097,16 +1087,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
@@ -1122,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1151,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1169,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -1181,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1208,48 +1198,45 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
       <c r="I4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
+      <c r="A5" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1257,19 +1244,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>733910060</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1277,39 +1267,45 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8">
-        <v>733910060</v>
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1317,22 +1313,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1340,22 +1336,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1363,76 +1359,52 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="E11">
+        <v>74438343022</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" t="s">
-        <v>30</v>
+      <c r="H11" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12">
+      <c r="A12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13">
-        <v>74438343022</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
+      <c r="J12" s="5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H13" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
changed battery from BT1 to B1
</commit_message>
<xml_diff>
--- a/sulu-reg/sulu_reg_bom.xlsx
+++ b/sulu-reg/sulu_reg_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2634F6A1-007B-4B80-B115-479EEFF4C22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F41D85-CD64-447C-86FD-5F712F94D75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="5460" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6150" yWindow="6150" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>https://www.digikey.com/en/products/detail/tdk-invensense/ICM-20948/6623535</t>
   </si>
   <si>
-    <t>BT1</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05B104KQ5NNNC/3887169</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>B1 (On Back)</t>
   </si>
 </sst>
 </file>
@@ -723,11 +723,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1090,7 +1091,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1141,7 +1142,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1159,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -1171,7 +1172,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1198,19 +1199,19 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -1221,22 +1222,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1244,13 +1245,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>733910060</v>
@@ -1259,7 +1260,7 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1267,22 +1268,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1290,22 +1291,22 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1313,22 +1314,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1336,22 +1337,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1359,13 +1360,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>74438343022</v>
@@ -1374,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1382,15 +1383,15 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>

</xml_diff>

<commit_message>
added headers to bom
</commit_message>
<xml_diff>
--- a/sulu-reg/sulu_reg_bom.xlsx
+++ b/sulu-reg/sulu_reg_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F41D85-CD64-447C-86FD-5F712F94D75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3A2E6-3694-44E2-87E9-81E46AF49940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6150" yWindow="6150" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -226,6 +226,39 @@
   </si>
   <si>
     <t>B1 (On Back)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC013DAAN-RC/2775281</t>
+  </si>
+  <si>
+    <t>PRPC013DAAN-RC</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 26POS 2.54MM</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 26 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC010SAAN-RC/2775244</t>
+  </si>
+  <si>
+    <t>S1011EC-10-ND</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 10 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 2.54MM</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,6 +1436,58 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H11" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>

</xml_diff>

<commit_message>
Generated Sulu v2.1 gerbers, drill files & updated BOM
</commit_message>
<xml_diff>
--- a/sulu-reg/sulu_reg_bom.xlsx
+++ b/sulu-reg/sulu_reg_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\sulu-reg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3A2E6-3694-44E2-87E9-81E46AF49940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B31216-D43D-4AE9-9300-5E88ABA581CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="6150" windowWidth="43200" windowHeight="23655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -228,30 +228,12 @@
     <t>B1 (On Back)</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC013DAAN-RC/2775281</t>
-  </si>
-  <si>
-    <t>PRPC013DAAN-RC</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>J1, J2</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 26POS 2.54MM</t>
-  </si>
-  <si>
-    <t>Connector Header Through Hole 26 position 0.100" (2.54mm)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC010SAAN-RC/2775244</t>
   </si>
   <si>
-    <t>S1011EC-10-ND</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -259,6 +241,39 @@
   </si>
   <si>
     <t>CONN HEADER VERT 10POS 2.54MM</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>PRPC010DAAN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC010DAAN-RC/2775284</t>
+  </si>
+  <si>
+    <t>PRPC010SAAN-RC</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 20POS 2.54MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC011DAAN-RC/2775283</t>
+  </si>
+  <si>
+    <t>PRPC011DAAN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 22POS 2.54MM</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 22 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 20 position 0.100" (2.54mm)</t>
   </si>
 </sst>
 </file>
@@ -756,14 +771,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1121,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,13 +1266,13 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>64</v>
       </c>
       <c r="E5" t="s">
@@ -1415,48 +1427,40 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="E12" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5">
+      <c r="I12">
         <v>1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="H13" t="s">
-        <v>65</v>
+      <c r="H13" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1467,32 +1471,61 @@
         <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="H14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14">
+      <c r="H15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H11" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{73A74E60-9B27-4247-83C4-FDB39D81F74E}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{FFAF6F37-C78D-4E15-BF8B-8AEC0802AEEA}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{0F26DF7E-51AF-44ED-A8C0-7FC658B4F702}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Sulu bom and component pos files for assembly
</commit_message>
<xml_diff>
--- a/sulu-reg/sulu_reg_bom.xlsx
+++ b/sulu-reg/sulu_reg_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B31216-D43D-4AE9-9300-5E88ABA581CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE26A37-BEA8-4F29-8E8E-6BAA726F5710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>Connector Header Through Hole 20 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Populate</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -771,11 +783,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="44" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1133,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,6 +1196,9 @@
       <c r="I1" t="s">
         <v>16</v>
       </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1210,37 +1228,45 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="J2" t="s">
+        <v>83</v>
+      </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>1</v>
       </c>
-      <c r="P3" s="1"/>
+      <c r="J3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1264,52 +1290,65 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>1</v>
       </c>
+      <c r="J5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>733910060</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>1</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1333,6 +1372,9 @@
       <c r="I7">
         <v>1</v>
       </c>
+      <c r="J7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1356,6 +1398,9 @@
       <c r="I8">
         <v>1</v>
       </c>
+      <c r="J8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1379,6 +1424,9 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1402,6 +1450,9 @@
       <c r="I10">
         <v>1</v>
       </c>
+      <c r="J10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1425,6 +1476,9 @@
       <c r="I11">
         <v>2</v>
       </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1439,83 +1493,106 @@
       <c r="I12">
         <v>1</v>
       </c>
+      <c r="J12" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>1</v>
       </c>
+      <c r="J13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <v>1</v>
       </c>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>1</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>